<commit_message>
update readme and features
</commit_message>
<xml_diff>
--- a/player_scores.xlsx
+++ b/player_scores.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.464166048872823</v>
+        <v>-0.5664960695472127</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>-0.3984099772007817</v>
+        <v>-0.4361400413227467</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.4600069830761218</v>
+        <v>-0.5371685250986227</v>
       </c>
     </row>
     <row r="5">
@@ -482,7 +482,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>-0.435984167819126</v>
+        <v>-0.4931828166462521</v>
       </c>
     </row>
     <row r="6">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.4892127044179342</v>
+        <v>-0.5571679912696158</v>
       </c>
     </row>
     <row r="7">
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>-0.4461916019838674</v>
+        <v>-0.5466931779871508</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>-0.4699866527567598</v>
+        <v>-0.5712379502829247</v>
       </c>
     </row>
     <row r="9">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>-0.6373595996764519</v>
+        <v>-0.7974733395810489</v>
       </c>
     </row>
     <row r="10">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>-0.4757890752019706</v>
+        <v>-0.5425470077601648</v>
       </c>
     </row>
     <row r="11">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>-0.360760635740233</v>
+        <v>-0.4026775245560015</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>-0.3099071932341287</v>
+        <v>-0.3404220649242103</v>
       </c>
     </row>
     <row r="13">
@@ -562,7 +562,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.4976656882843148</v>
+        <v>-0.5464065075226781</v>
       </c>
     </row>
     <row r="14">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.3536759129510049</v>
+        <v>0.4144728952908346</v>
       </c>
     </row>
     <row r="15">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.02960780936950459</v>
+        <v>0.02358490778145368</v>
       </c>
     </row>
     <row r="16">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.006298617260136434</v>
+        <v>-0.05931516769736236</v>
       </c>
     </row>
     <row r="17">
@@ -602,7 +602,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.149713785102596</v>
+        <v>0.2266109970553055</v>
       </c>
     </row>
     <row r="18">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>-0.1523768344367138</v>
+        <v>-0.2077798954074883</v>
       </c>
     </row>
     <row r="19">
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>-0.2330646825437304</v>
+        <v>-0.3069793719305974</v>
       </c>
     </row>
     <row r="20">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01245290532835157</v>
+        <v>0.01155715253908448</v>
       </c>
     </row>
     <row r="21">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.2475367277831189</v>
+        <v>0.284731672537188</v>
       </c>
     </row>
     <row r="22">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.003673258957774855</v>
+        <v>-0.005243094914738989</v>
       </c>
     </row>
     <row r="23">
@@ -662,7 +662,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.06344214927737966</v>
+        <v>0.06392999676223968</v>
       </c>
     </row>
     <row r="24">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.1027674164725638</v>
+        <v>0.09990703194902172</v>
       </c>
     </row>
     <row r="25">
@@ -682,7 +682,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>-0.2103356695292164</v>
+        <v>-0.2512958655336935</v>
       </c>
     </row>
     <row r="26">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-0.1307941845594041</v>
+        <v>-0.1658123980933962</v>
       </c>
     </row>
     <row r="27">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-0.0314744114039849</v>
+        <v>-0.03741110982631637</v>
       </c>
     </row>
     <row r="28">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.2397783000876597</v>
+        <v>0.2179162127468129</v>
       </c>
     </row>
     <row r="29">
@@ -722,7 +722,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>-0.08578685032624071</v>
+        <v>-0.1275363987006121</v>
       </c>
     </row>
     <row r="30">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-0.4407548241918118</v>
+        <v>-0.09421348167506201</v>
       </c>
     </row>
     <row r="31">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-0.3853257485558281</v>
+        <v>0.118423199919853</v>
       </c>
     </row>
     <row r="32">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>-0.6844893754755602</v>
+        <v>-0.1920792050671807</v>
       </c>
     </row>
     <row r="33">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-0.7232679864674635</v>
+        <v>-0.1776041784525154</v>
       </c>
     </row>
     <row r="34">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>-0.03411468818855912</v>
+        <v>-0.07279364689780141</v>
       </c>
     </row>
     <row r="35">
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0.01656219181492859</v>
+        <v>-0.01510879135064917</v>
       </c>
     </row>
     <row r="36">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>-0.08067214871070273</v>
+        <v>-0.1994933507736878</v>
       </c>
     </row>
     <row r="37">
@@ -802,7 +802,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>0.1780679065827405</v>
+        <v>0.23605657102707</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>-0.2350671321082697</v>
+        <v>-0.3022795516967504</v>
       </c>
     </row>
     <row r="39">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>-0.5083779096357114</v>
+        <v>-0.6571408764479121</v>
       </c>
     </row>
     <row r="40">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>-0.2056863082143626</v>
+        <v>-0.2823974595631665</v>
       </c>
     </row>
     <row r="41">
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>-0.1352527216906279</v>
+        <v>-0.1753352089740312</v>
       </c>
     </row>
     <row r="42">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>-0.2413442994124286</v>
+        <v>-0.3147999646388679</v>
       </c>
     </row>
     <row r="43">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>-0.1256730362629826</v>
+        <v>-0.1847239898599183</v>
       </c>
     </row>
     <row r="44">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>-0.1644724629061</v>
+        <v>-0.2340311456644844</v>
       </c>
     </row>
     <row r="45">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>-0.2000440317723206</v>
+        <v>-0.2412528006065553</v>
       </c>
     </row>
     <row r="46">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>-0.20052010214032</v>
+        <v>-0.2751932964850113</v>
       </c>
     </row>
     <row r="47">
@@ -902,7 +902,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>-0.5253289862384857</v>
+        <v>-0.6284685788168278</v>
       </c>
     </row>
     <row r="48">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>-0.2953996642804925</v>
+        <v>-0.374323726930951</v>
       </c>
     </row>
     <row r="49">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>-0.210645659825496</v>
+        <v>-0.2519311507540934</v>
       </c>
     </row>
     <row r="50">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>0.06519086747627874</v>
+        <v>0.07433946178030867</v>
       </c>
     </row>
     <row r="51">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>-0.1100883899693778</v>
+        <v>-0.1366867419062487</v>
       </c>
     </row>
     <row r="52">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>-0.00432275699693171</v>
+        <v>-0.01172748182599049</v>
       </c>
     </row>
     <row r="53">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>-0.006066884242245741</v>
+        <v>-0.002100530557000856</v>
       </c>
     </row>
     <row r="54">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>0.002527146485445734</v>
+        <v>-0.0009408250518614793</v>
       </c>
     </row>
     <row r="55">
@@ -982,7 +982,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0.1696624346516327</v>
+        <v>0.1976166453420277</v>
       </c>
     </row>
     <row r="56">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>-0.02234714869594881</v>
+        <v>-0.009501117240594794</v>
       </c>
     </row>
     <row r="57">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>-0.005764373680387764</v>
+        <v>-0.01564762683657516</v>
       </c>
     </row>
     <row r="58">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>-0.04172307743603748</v>
+        <v>-0.0414926571274016</v>
       </c>
     </row>
     <row r="59">
@@ -1022,7 +1022,7 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>0.01578783043471924</v>
+        <v>0.006632197058229857</v>
       </c>
     </row>
     <row r="60">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>-0.002249098787985949</v>
+        <v>0.01688795277747085</v>
       </c>
     </row>
     <row r="61">
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>0.001133015982717184</v>
+        <v>0.007894357705547264</v>
       </c>
     </row>
     <row r="62">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>0.1126976011570995</v>
+        <v>0.1296776238540422</v>
       </c>
     </row>
     <row r="63">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0.1528070951582878</v>
+        <v>0.2130853869571952</v>
       </c>
     </row>
     <row r="64">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="B64" t="n">
-        <v>-0.1734205000916381</v>
+        <v>-0.203853777179843</v>
       </c>
     </row>
     <row r="65">
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0.009941892696336632</v>
+        <v>-0.008382073170275468</v>
       </c>
     </row>
     <row r="66">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>-0.04668933699786201</v>
+        <v>-0.0143028176851671</v>
       </c>
     </row>
     <row r="67">
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>0.05144211078360529</v>
+        <v>0.03231732722739699</v>
       </c>
     </row>
     <row r="68">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0.02895969751174944</v>
+        <v>0.01093885602750555</v>
       </c>
     </row>
     <row r="69">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>-0.002270698088294562</v>
+        <v>0.02703306490989708</v>
       </c>
     </row>
     <row r="70">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>0.1980178943517202</v>
+        <v>0.2455166095388436</v>
       </c>
     </row>
     <row r="71">
@@ -1142,7 +1142,7 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>-0.07193841207961461</v>
+        <v>-0.07134232224975101</v>
       </c>
     </row>
     <row r="72">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>0.354351283233619</v>
+        <v>0.4310516329957331</v>
       </c>
     </row>
     <row r="73">
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>0.1674214645628746</v>
+        <v>0.2263222698669136</v>
       </c>
     </row>
     <row r="74">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>0.1947080725430437</v>
+        <v>0.2093110868181786</v>
       </c>
     </row>
     <row r="75">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>0.3729129749871956</v>
+        <v>0.4367228708906591</v>
       </c>
     </row>
     <row r="76">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>0.1671220651761864</v>
+        <v>0.2066625670401257</v>
       </c>
     </row>
     <row r="77">
@@ -1202,7 +1202,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>-0.1846445951701957</v>
+        <v>-0.2089765009323316</v>
       </c>
     </row>
     <row r="78">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>-0.07065733796800952</v>
+        <v>-0.08127697723661732</v>
       </c>
     </row>
     <row r="79">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>0.3673686078612601</v>
+        <v>0.4357946272645412</v>
       </c>
     </row>
     <row r="80">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>0.0199929755501173</v>
+        <v>0.02589980063020375</v>
       </c>
     </row>
     <row r="81">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>0.1815077298775178</v>
+        <v>0.1986133481052239</v>
       </c>
     </row>
     <row r="82">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>0.1016691234148727</v>
+        <v>0.1303470659471042</v>
       </c>
     </row>
     <row r="83">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="B83" t="n">
-        <v>0.02188789142547195</v>
+        <v>0.01094085719139458</v>
       </c>
     </row>
     <row r="84">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>0.1414572889491003</v>
+        <v>0.173748220711727</v>
       </c>
     </row>
     <row r="85">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>0.2224934815288248</v>
+        <v>0.2504041201479615</v>
       </c>
     </row>
     <row r="86">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>0.1156755740328043</v>
+        <v>0.1202593546188853</v>
       </c>
     </row>
     <row r="87">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>0.2067906625384087</v>
+        <v>0.2675351494061741</v>
       </c>
     </row>
     <row r="88">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0.2500134056613844</v>
+        <v>0.3570341646186974</v>
       </c>
     </row>
     <row r="89">
@@ -1322,7 +1322,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>0.01586978864264958</v>
+        <v>0.04941819241653365</v>
       </c>
     </row>
     <row r="90">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>0.310923302794116</v>
+        <v>0.3670699540512709</v>
       </c>
     </row>
     <row r="91">
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0.2111756487665515</v>
+        <v>0.272985159173188</v>
       </c>
     </row>
     <row r="92">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>0.189062807646851</v>
+        <v>0.2312854247614052</v>
       </c>
     </row>
     <row r="93">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>0.03745853726282231</v>
+        <v>0.03638017565047692</v>
       </c>
     </row>
     <row r="94">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>0.09345657888429684</v>
+        <v>0.1161180873737637</v>
       </c>
     </row>
     <row r="95">
@@ -1382,7 +1382,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>0.02611489547469888</v>
+        <v>0.05748720845702045</v>
       </c>
     </row>
     <row r="96">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>-0.05753438087088573</v>
+        <v>-0.0215153756233217</v>
       </c>
     </row>
     <row r="97">
@@ -1402,7 +1402,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>0.121737998838353</v>
+        <v>0.1617353827136256</v>
       </c>
     </row>
     <row r="98">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0.4393450536040618</v>
+        <v>0.5533821121420188</v>
       </c>
     </row>
     <row r="99">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>0.3937109204511526</v>
+        <v>0.484205464036842</v>
       </c>
     </row>
     <row r="100">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.3296249460008679</v>
+        <v>0.4236925397683906</v>
       </c>
     </row>
     <row r="101">
@@ -1442,7 +1442,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>0.6052494019188217</v>
+        <v>0.7454669809451054</v>
       </c>
     </row>
     <row r="102">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0.2684843188480225</v>
+        <v>0.3310542140074799</v>
       </c>
     </row>
     <row r="103">
@@ -1462,7 +1462,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>0.1972544002106251</v>
+        <v>0.2631345108208606</v>
       </c>
     </row>
     <row r="104">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="B104" t="n">
-        <v>0.2654742093499664</v>
+        <v>0.3185023476819153</v>
       </c>
     </row>
     <row r="105">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>0.1102898117175646</v>
+        <v>0.0979728812981268</v>
       </c>
     </row>
     <row r="106">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>0.380081662950887</v>
+        <v>0.449268492969307</v>
       </c>
     </row>
     <row r="107">
@@ -1502,7 +1502,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>0.5784902652760773</v>
+        <v>0.6822795084745374</v>
       </c>
     </row>
     <row r="108">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0.4288642941828438</v>
+        <v>0.5029500087637681</v>
       </c>
     </row>
     <row r="109">
@@ -1522,7 +1522,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>0.2282802062467807</v>
+        <v>0.2975128394246513</v>
       </c>
     </row>
     <row r="110">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0.2182323527909451</v>
+        <v>0.2694575730101699</v>
       </c>
     </row>
     <row r="111">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>0.00802901684865596</v>
+        <v>-0.07754066984257242</v>
       </c>
     </row>
     <row r="112">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>-0.07179186658756703</v>
+        <v>-0.0477600149143873</v>
       </c>
     </row>
     <row r="113">
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>0.1157556522322082</v>
+        <v>0.1755379928819636</v>
       </c>
     </row>
     <row r="114">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>-0.1156367600700451</v>
+        <v>-0.1004729398308437</v>
       </c>
     </row>
     <row r="115">
@@ -1582,7 +1582,7 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>0.1190398640927868</v>
+        <v>0.162615240589367</v>
       </c>
     </row>
     <row r="116">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0.06635789982926969</v>
+        <v>0.1038539838732898</v>
       </c>
     </row>
     <row r="117">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>0.1703712074423696</v>
+        <v>0.1141277493459276</v>
       </c>
     </row>
     <row r="118">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>0.1183846204186655</v>
+        <v>0.1057233991064729</v>
       </c>
     </row>
     <row r="119">
@@ -1622,7 +1622,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0.003101643213907115</v>
+        <v>-0.07370327716450033</v>
       </c>
     </row>
     <row r="120">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>-0.07047765917623737</v>
+        <v>-0.06244402007442865</v>
       </c>
     </row>
     <row r="121">
@@ -1642,7 +1642,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>0.1617621524779151</v>
+        <v>0.2121881080823664</v>
       </c>
     </row>
     <row r="122">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>-0.2641171874545835</v>
+        <v>-0.3764873681567382</v>
       </c>
     </row>
     <row r="123">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="B123" t="n">
-        <v>-0.3104663637482779</v>
+        <v>-0.373037751830464</v>
       </c>
     </row>
     <row r="124">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>-0.3400076428205118</v>
+        <v>-0.3978231460803199</v>
       </c>
     </row>
     <row r="125">
@@ -1682,7 +1682,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>-0.3504107322072049</v>
+        <v>-0.4605336321505669</v>
       </c>
     </row>
     <row r="126">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>-0.3611252638287954</v>
+        <v>-0.4380338817586157</v>
       </c>
     </row>
     <row r="127">
@@ -1702,7 +1702,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>-0.3545298334560165</v>
+        <v>-0.4731803917823798</v>
       </c>
     </row>
     <row r="128">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="B128" t="n">
-        <v>-0.3052254692710486</v>
+        <v>-0.3206905203920072</v>
       </c>
     </row>
     <row r="129">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>-0.4181035758450106</v>
+        <v>-0.4985917344926163</v>
       </c>
     </row>
     <row r="130">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>-0.5045941823741216</v>
+        <v>-0.5868984659402303</v>
       </c>
     </row>
     <row r="131">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>-0.2414661138362109</v>
+        <v>-0.3179646442813064</v>
       </c>
     </row>
     <row r="132">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>-0.502399560172024</v>
+        <v>-0.6394334570414045</v>
       </c>
     </row>
     <row r="133">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>-0.3542635532871392</v>
+        <v>-0.3912465695228383</v>
       </c>
     </row>
     <row r="134">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>0.3847383820758238</v>
+        <v>0.4905996676788515</v>
       </c>
     </row>
     <row r="135">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>0.775439638834488</v>
+        <v>0.4025874100312921</v>
       </c>
     </row>
     <row r="136">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>0.2457239211408184</v>
+        <v>0.3305835078702661</v>
       </c>
     </row>
     <row r="137">
@@ -1802,7 +1802,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>0.3330861626035298</v>
+        <v>0.3988252963059269</v>
       </c>
     </row>
     <row r="138">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>0.6381606724008132</v>
+        <v>0.146418781965773</v>
       </c>
     </row>
     <row r="139">
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.9290304813240534</v>
+        <v>0.4076768932778474</v>
       </c>
     </row>
     <row r="140">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.1015693114377842</v>
+        <v>0.132698968441055</v>
       </c>
     </row>
     <row r="141">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.1926133472922383</v>
+        <v>0.2729028605682403</v>
       </c>
     </row>
     <row r="142">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.7642306982789071</v>
+        <v>0.4783126136697041</v>
       </c>
     </row>
     <row r="143">
@@ -1862,7 +1862,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>0.4400592648626546</v>
+        <v>0.59175860304156</v>
       </c>
     </row>
     <row r="144">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>0.4739231538382109</v>
+        <v>0.5909453997744539</v>
       </c>
     </row>
     <row r="145">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>0.3974322425595987</v>
+        <v>0.4844257811259522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>